<commit_message>
Lots of writing and figures
</commit_message>
<xml_diff>
--- a/Paper/Supplemental File 1_v2.xlsx
+++ b/Paper/Supplemental File 1_v2.xlsx
@@ -19634,8 +19634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N707"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" topLeftCell="A223" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D232" sqref="D232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>